<commit_message>
updated files and slides
</commit_message>
<xml_diff>
--- a/Schaefer_MLE.xlsx
+++ b/Schaefer_MLE.xlsx
@@ -117,7 +117,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="129"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -156,8 +155,38 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -165,9 +194,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -668,130 +727,130 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="42"/>
                 <c:pt idx="0">
-                  <c:v>96.15116202790905</c:v>
+                  <c:v>96.17083548407005</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.74425367953777</c:v>
+                  <c:v>74.97053094477242</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>57.24083055022226</c:v>
+                  <c:v>57.66760369091573</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>46.41847271268431</c:v>
+                  <c:v>46.98707779000384</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>39.02187099606867</c:v>
+                  <c:v>39.73810048266694</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>38.1993331260412</c:v>
+                  <c:v>38.98158515275204</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42.87357301573827</c:v>
+                  <c:v>43.59906271402094</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>44.9269213740342</c:v>
+                  <c:v>45.61108369233584</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>44.03854335649626</c:v>
+                  <c:v>44.73251267637495</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>44.52009063615211</c:v>
+                  <c:v>45.19747341522991</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>46.95166023412025</c:v>
+                  <c:v>47.55453448057372</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>49.40096812555013</c:v>
+                  <c:v>49.89539792994903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>54.41611101061322</c:v>
+                  <c:v>54.69899870024786</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>58.46697979816075</c:v>
+                  <c:v>58.50268349577161</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>53.73176704442783</c:v>
+                  <c:v>53.69811277139616</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>41.50145468344261</c:v>
+                  <c:v>41.60464002401348</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>33.31024851219898</c:v>
+                  <c:v>33.52012630168254</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>30.24145977334243</c:v>
+                  <c:v>30.48385229188815</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>29.34386358118735</c:v>
+                  <c:v>29.58663079351279</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>29.27248331045151</c:v>
+                  <c:v>29.49852484683861</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>26.15101757239115</c:v>
+                  <c:v>26.43524815016829</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>23.63059291411923</c:v>
+                  <c:v>23.99186662240851</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>21.56819183311879</c:v>
+                  <c:v>22.03301538271435</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23.14283184304033</c:v>
+                  <c:v>23.66511085853851</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>32.09817009468764</c:v>
+                  <c:v>32.49406447415657</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>44.82125933971611</c:v>
+                  <c:v>44.89895851232576</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>60.3603883777475</c:v>
+                  <c:v>59.91112399136667</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>76.11030699392542</c:v>
+                  <c:v>75.01953005483978</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>89.47989423476778</c:v>
+                  <c:v>87.79709178144682</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>98.7539857292362</c:v>
+                  <c:v>96.67707196684721</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>103.2217950715925</c:v>
+                  <c:v>100.992162674857</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>107.1492185943532</c:v>
+                  <c:v>104.8479183661444</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>110.4058466983586</c:v>
+                  <c:v>108.1062858916806</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>111.5840240548066</c:v>
+                  <c:v>109.3740653545703</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>112.4040945740298</c:v>
+                  <c:v>110.2845093751125</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>119.2882088601692</c:v>
+                  <c:v>117.0870735609116</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>128.7760380548626</c:v>
+                  <c:v>126.5190500881075</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>129.8880933886176</c:v>
+                  <c:v>127.899670614749</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>129.8166398410997</c:v>
+                  <c:v>128.0456923124284</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>130.7949734895872</c:v>
+                  <c:v>129.1325981513057</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>131.8805424531792</c:v>
+                  <c:v>130.2911354708765</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>135.6883839921741</c:v>
+                  <c:v>134.0796870494855</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -806,11 +865,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2136567320"/>
-        <c:axId val="2136612664"/>
+        <c:axId val="2076524248"/>
+        <c:axId val="2076527288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2136567320"/>
+        <c:axId val="2076524248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -820,12 +879,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136612664"/>
+        <c:crossAx val="2076527288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2136612664"/>
+        <c:axId val="2076527288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -836,7 +895,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136567320"/>
+        <c:crossAx val="2076524248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1076,154 +1135,154 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="50"/>
                 <c:pt idx="0">
-                  <c:v>151.0837712652826</c:v>
+                  <c:v>179.8530088901964</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>146.4098042241332</c:v>
+                  <c:v>159.4889943662231</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>140.2661094149722</c:v>
+                  <c:v>147.9143709222627</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>135.2286276384028</c:v>
+                  <c:v>140.4761680232324</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>127.9589413768424</c:v>
+                  <c:v>131.9569098316909</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>121.2281427503124</c:v>
+                  <c:v>124.4926780875793</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>106.143214324641</c:v>
+                  <c:v>108.915264918993</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>84.29631296013445</c:v>
+                  <c:v>86.67169887445353</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>63.74412709042717</c:v>
+                  <c:v>65.79924980415613</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>49.62857149649301</c:v>
+                  <c:v>51.48195565046672</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42.30907974186597</c:v>
+                  <c:v>44.07778276935386</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.97866706770226</c:v>
+                  <c:v>36.73938369491305</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>40.6799395438891</c:v>
+                  <c:v>42.53922343692751</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>44.2365898658809</c:v>
+                  <c:v>46.13015598099293</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>44.7468554548101</c:v>
+                  <c:v>46.63116120846236</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42.47704493535782</c:v>
+                  <c:v>44.34336649721875</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>45.7006206966312</c:v>
+                  <c:v>47.57677282489532</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>47.29307580831465</c:v>
+                  <c:v>49.13702784918552</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>50.55178450142624</c:v>
+                  <c:v>52.33749235502991</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>57.22620006967092</c:v>
+                  <c:v>58.90632729646163</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>58.57504205466603</c:v>
+                  <c:v>60.073217605197</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>47.84751280895962</c:v>
+                  <c:v>49.13505520985143</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>34.35136284530701</c:v>
+                  <c:v>35.47817686884856</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>31.62379384141367</c:v>
+                  <c:v>32.69321517863866</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>28.27323893667398</c:v>
+                  <c:v>29.30316953079745</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>29.84599115113509</c:v>
+                  <c:v>30.86849536795853</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>28.13186128995924</c:v>
+                  <c:v>29.12398449496602</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>23.66353378864069</c:v>
+                  <c:v>24.63857144824581</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>23.13984174121086</c:v>
+                  <c:v>24.15476932699874</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>19.57868781638577</c:v>
+                  <c:v>20.6547673711951</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>26.25861527247728</c:v>
+                  <c:v>27.47403547593788</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>37.31586693465743</c:v>
+                  <c:v>38.61060837496743</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>51.45830137426284</c:v>
+                  <c:v>52.70242773116397</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>68.09307571722901</c:v>
+                  <c:v>69.14152610310506</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>82.6530055544161</c:v>
+                  <c:v>83.42907427467531</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>94.57323279946527</c:v>
+                  <c:v>95.12782943728355</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>101.0215157518246</c:v>
+                  <c:v>101.4886903138447</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>103.4222938114359</c:v>
+                  <c:v>103.9036239473847</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>108.8002743580342</c:v>
+                  <c:v>109.3303144922383</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>109.8724573205267</c:v>
+                  <c:v>110.5303128810414</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>111.1338035020134</c:v>
+                  <c:v>111.9086547412147</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>111.4967106184297</c:v>
+                  <c:v>112.3819239311632</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>124.7686618102908</c:v>
+                  <c:v>125.7433362058556</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>130.2885553417585</c:v>
+                  <c:v>131.5641598162914</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>126.9712279323034</c:v>
+                  <c:v>128.5511664133977</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>130.1470325611167</c:v>
+                  <c:v>131.8611307259577</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>128.9089413578642</c:v>
+                  <c:v>130.7616558188951</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>132.2971390798656</c:v>
+                  <c:v>134.2173003031036</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>136.4508527333194</c:v>
+                  <c:v>138.4666039635718</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>124.9963674306884</c:v>
+                  <c:v>127.1380205674877</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1571,11 +1630,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2136824296"/>
-        <c:axId val="2136751592"/>
+        <c:axId val="2076031112"/>
+        <c:axId val="2076034168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2136824296"/>
+        <c:axId val="2076031112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1585,12 +1644,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136751592"/>
+        <c:crossAx val="2076034168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2136751592"/>
+        <c:axId val="2076034168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1601,7 +1660,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2136824296"/>
+        <c:crossAx val="2076031112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2038,7 +2097,7 @@
       </c>
       <c r="C5">
         <f>InitBio</f>
-        <v>151.08377126528265</v>
+        <v>179.85300889019641</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2049,8 +2108,8 @@
         <v>7.0259999999999998</v>
       </c>
       <c r="C6">
-        <f>C5+C5*growth_rate*(1-C5/K)-B5</f>
-        <v>146.40980422413324</v>
+        <f t="shared" ref="C6:C37" si="0">C5+C5*growth_rate*(1-C5/K)-B5</f>
+        <v>159.4889943662231</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2061,8 +2120,8 @@
         <v>8.8780000000000001</v>
       </c>
       <c r="C7">
-        <f>C6+C6*growth_rate*(1-C6/K)-B6</f>
-        <v>140.26610941497225</v>
+        <f t="shared" si="0"/>
+        <v>147.91437092226275</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2073,8 +2132,8 @@
         <v>13.34</v>
       </c>
       <c r="C8">
-        <f>C7+C7*growth_rate*(1-C7/K)-B7</f>
-        <v>135.22862763840283</v>
+        <f t="shared" si="0"/>
+        <v>140.47616802323245</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -2085,8 +2144,8 @@
         <v>15.708</v>
       </c>
       <c r="C9">
-        <f>C8+C8*growth_rate*(1-C8/K)-B8</f>
-        <v>127.9589413768424</v>
+        <f t="shared" si="0"/>
+        <v>131.95690983169089</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -2097,8 +2156,8 @@
         <v>26.425999999999998</v>
       </c>
       <c r="C10">
-        <f>C9+C9*growth_rate*(1-C9/K)-B9</f>
-        <v>121.2281427503124</v>
+        <f t="shared" si="0"/>
+        <v>124.49267808757929</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2109,8 +2168,8 @@
         <v>37.341999999999999</v>
       </c>
       <c r="C11">
-        <f>C10+C10*growth_rate*(1-C10/K)-B10</f>
-        <v>106.14321432464097</v>
+        <f t="shared" si="0"/>
+        <v>108.91526491899292</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2121,8 +2180,8 @@
         <v>39.259</v>
       </c>
       <c r="C12">
-        <f>C11+C11*growth_rate*(1-C11/K)-B11</f>
-        <v>84.296312960134458</v>
+        <f t="shared" si="0"/>
+        <v>86.671698874453526</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2133,8 +2192,8 @@
         <v>32.814999999999998</v>
       </c>
       <c r="C13">
-        <f>C12+C12*growth_rate*(1-C12/K)-B12</f>
-        <v>63.74412709042717</v>
+        <f t="shared" si="0"/>
+        <v>65.799249804156133</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2145,8 +2204,8 @@
         <v>24.312999999999999</v>
       </c>
       <c r="C14">
-        <f>C13+C13*growth_rate*(1-C13/K)-B13</f>
-        <v>49.628571496493009</v>
+        <f t="shared" si="0"/>
+        <v>51.481955650466716</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2157,8 +2216,8 @@
         <v>22.893999999999998</v>
       </c>
       <c r="C15">
-        <f>C14+C14*growth_rate*(1-C14/K)-B14</f>
-        <v>42.309079741865972</v>
+        <f t="shared" si="0"/>
+        <v>44.07778276935386</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2169,8 +2228,8 @@
         <v>8.0570000000000004</v>
       </c>
       <c r="C16">
-        <f>C15+C15*growth_rate*(1-C15/K)-B15</f>
-        <v>34.978667067702261</v>
+        <f t="shared" si="0"/>
+        <v>36.739383694913052</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2181,8 +2240,8 @@
         <v>11.638</v>
       </c>
       <c r="C17">
-        <f>C16+C16*growth_rate*(1-C16/K)-B16</f>
-        <v>40.679939543889098</v>
+        <f t="shared" si="0"/>
+        <v>42.539223436927514</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2193,8 +2252,8 @@
         <v>15.465999999999999</v>
       </c>
       <c r="C18">
-        <f>C17+C17*growth_rate*(1-C17/K)-B17</f>
-        <v>44.236589865880894</v>
+        <f t="shared" si="0"/>
+        <v>46.130155980992939</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2205,8 +2264,8 @@
         <v>18.350999999999999</v>
       </c>
       <c r="C19">
-        <f>C18+C18*growth_rate*(1-C18/K)-B18</f>
-        <v>44.746855454810095</v>
+        <f t="shared" si="0"/>
+        <v>46.631161208462359</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2217,8 +2276,8 @@
         <v>12.377000000000001</v>
       </c>
       <c r="C20">
-        <f>C19+C19*growth_rate*(1-C19/K)-B19</f>
-        <v>42.477044935357824</v>
+        <f t="shared" si="0"/>
+        <v>44.343366497218746</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2229,8 +2288,8 @@
         <v>14.68</v>
       </c>
       <c r="C21">
-        <f>C20+C20*growth_rate*(1-C20/K)-B20</f>
-        <v>45.700620696631205</v>
+        <f t="shared" si="0"/>
+        <v>47.576772824895322</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2241,8 +2300,8 @@
         <v>13.319000000000001</v>
       </c>
       <c r="C22">
-        <f>C21+C21*growth_rate*(1-C21/K)-B21</f>
-        <v>47.293075808314654</v>
+        <f t="shared" si="0"/>
+        <v>49.137027849185522</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2253,8 +2312,8 @@
         <v>10.473000000000001</v>
       </c>
       <c r="C23">
-        <f>C22+C22*growth_rate*(1-C22/K)-B22</f>
-        <v>50.551784501426241</v>
+        <f t="shared" si="0"/>
+        <v>52.337492355029909</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2265,8 +2324,8 @@
         <v>16.734999999999999</v>
       </c>
       <c r="C24">
-        <f>C23+C23*growth_rate*(1-C23/K)-B23</f>
-        <v>57.226200069670924</v>
+        <f t="shared" si="0"/>
+        <v>58.906327296461626</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2277,8 +2336,8 @@
         <v>28.963000000000001</v>
       </c>
       <c r="C25">
-        <f>C24+C24*growth_rate*(1-C24/K)-B24</f>
-        <v>58.575042054666028</v>
+        <f t="shared" si="0"/>
+        <v>60.073217605197001</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2289,8 +2348,8 @@
         <v>30.175999999999998</v>
       </c>
       <c r="C26">
-        <f>C25+C25*growth_rate*(1-C25/K)-B25</f>
-        <v>47.847512808959628</v>
+        <f t="shared" si="0"/>
+        <v>49.135055209851437</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2301,8 +2360,8 @@
         <v>16.314</v>
       </c>
       <c r="C27">
-        <f>C26+C26*growth_rate*(1-C26/K)-B26</f>
-        <v>34.351362845307008</v>
+        <f t="shared" si="0"/>
+        <v>35.478176868848564</v>
       </c>
     </row>
     <row r="28" spans="1:3">
@@ -2313,8 +2372,8 @@
         <v>16.158000000000001</v>
       </c>
       <c r="C28">
-        <f>C27+C27*growth_rate*(1-C27/K)-B27</f>
-        <v>31.623793841413672</v>
+        <f t="shared" si="0"/>
+        <v>32.69321517863866</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2325,8 +2384,8 @@
         <v>10.207000000000001</v>
       </c>
       <c r="C29">
-        <f>C28+C28*growth_rate*(1-C28/K)-B28</f>
-        <v>28.273238936673977</v>
+        <f t="shared" si="0"/>
+        <v>29.303169530797447</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2337,8 +2396,8 @@
         <v>13.986000000000001</v>
       </c>
       <c r="C30">
-        <f>C29+C29*growth_rate*(1-C29/K)-B29</f>
-        <v>29.845991151135088</v>
+        <f t="shared" si="0"/>
+        <v>30.868495367958531</v>
       </c>
     </row>
     <row r="31" spans="1:3">
@@ -2349,8 +2408,8 @@
         <v>16.202999999999999</v>
       </c>
       <c r="C31">
-        <f>C30+C30*growth_rate*(1-C30/K)-B30</f>
-        <v>28.131861289959243</v>
+        <f t="shared" si="0"/>
+        <v>29.12398449496602</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2361,8 +2420,8 @@
         <v>10.762</v>
       </c>
       <c r="C32">
-        <f>C31+C31*growth_rate*(1-C31/K)-B31</f>
-        <v>23.663533788640688</v>
+        <f t="shared" si="0"/>
+        <v>24.638571448245809</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2373,8 +2432,8 @@
         <v>13.615</v>
       </c>
       <c r="C33">
-        <f>C32+C32*growth_rate*(1-C32/K)-B32</f>
-        <v>23.139841741210866</v>
+        <f t="shared" si="0"/>
+        <v>24.154769326998739</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2385,8 +2444,8 @@
         <v>2.069</v>
       </c>
       <c r="C34">
-        <f>C33+C33*growth_rate*(1-C33/K)-B33</f>
-        <v>19.578687816385774</v>
+        <f t="shared" si="0"/>
+        <v>20.654767371195099</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2397,8 +2456,8 @@
         <v>6.7000000000000004E-2</v>
       </c>
       <c r="C35">
-        <f>C34+C34*growth_rate*(1-C34/K)-B34</f>
-        <v>26.258615272477282</v>
+        <f t="shared" si="0"/>
+        <v>27.474035475937878</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2409,8 +2468,8 @@
         <v>0.23200000000000001</v>
       </c>
       <c r="C36">
-        <f>C35+C35*growth_rate*(1-C35/K)-B35</f>
-        <v>37.315866934657429</v>
+        <f t="shared" si="0"/>
+        <v>38.610608374967434</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2421,8 +2480,8 @@
         <v>0.65800000000000003</v>
       </c>
       <c r="C37">
-        <f>C36+C36*growth_rate*(1-C36/K)-B36</f>
-        <v>51.458301374262838</v>
+        <f t="shared" si="0"/>
+        <v>52.702427731163972</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -2433,8 +2492,8 @@
         <v>4.3860000000000001</v>
       </c>
       <c r="C38">
-        <f>C37+C37*growth_rate*(1-C37/K)-B37</f>
-        <v>68.093075717229013</v>
+        <f t="shared" ref="C38:C54" si="1">C37+C37*growth_rate*(1-C37/K)-B37</f>
+        <v>69.141526103105065</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -2445,8 +2504,8 @@
         <v>6.8940000000000001</v>
       </c>
       <c r="C39">
-        <f>C38+C38*growth_rate*(1-C38/K)-B38</f>
-        <v>82.653005554416097</v>
+        <f t="shared" si="1"/>
+        <v>83.429074274675315</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2457,8 +2516,8 @@
         <v>11.161</v>
       </c>
       <c r="C40">
-        <f>C39+C39*growth_rate*(1-C39/K)-B39</f>
-        <v>94.573232799465274</v>
+        <f t="shared" si="1"/>
+        <v>95.127829437283552</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -2469,8 +2528,8 @@
         <v>14.145</v>
       </c>
       <c r="C41">
-        <f>C40+C40*growth_rate*(1-C40/K)-B40</f>
-        <v>101.02151575182459</v>
+        <f t="shared" si="1"/>
+        <v>101.48869031384466</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -2481,8 +2540,8 @@
         <v>10.698</v>
       </c>
       <c r="C42">
-        <f>C41+C41*growth_rate*(1-C41/K)-B41</f>
-        <v>103.42229381143589</v>
+        <f t="shared" si="1"/>
+        <v>103.90362394738474</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -2493,8 +2552,8 @@
         <v>13.805999999999999</v>
       </c>
       <c r="C43">
-        <f>C42+C42*growth_rate*(1-C42/K)-B42</f>
-        <v>108.80027435803422</v>
+        <f t="shared" si="1"/>
+        <v>109.33031449223827</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -2505,8 +2564,8 @@
         <v>13.353999999999999</v>
       </c>
       <c r="C44">
-        <f>C43+C43*growth_rate*(1-C43/K)-B43</f>
-        <v>109.87245732052675</v>
+        <f t="shared" si="1"/>
+        <v>110.53031288104141</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -2517,8 +2576,8 @@
         <v>13.933</v>
       </c>
       <c r="C45">
-        <f>C44+C44*growth_rate*(1-C44/K)-B44</f>
-        <v>111.13380350201335</v>
+        <f t="shared" si="1"/>
+        <v>111.9086547412147</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -2529,8 +2588,8 @@
         <v>0.93</v>
       </c>
       <c r="C46">
-        <f>C45+C45*growth_rate*(1-C45/K)-B45</f>
-        <v>111.49671061842974</v>
+        <f t="shared" si="1"/>
+        <v>112.38192393116319</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -2541,8 +2600,8 @@
         <v>4.617</v>
       </c>
       <c r="C47">
-        <f>C46+C46*growth_rate*(1-C46/K)-B46</f>
-        <v>124.76866181029082</v>
+        <f t="shared" si="1"/>
+        <v>125.7433362058556</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -2553,8 +2612,8 @@
         <v>11.403</v>
       </c>
       <c r="C48">
-        <f>C47+C47*growth_rate*(1-C47/K)-B47</f>
-        <v>130.2885553417585</v>
+        <f t="shared" si="1"/>
+        <v>131.56415981629144</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -2565,8 +2624,8 @@
         <v>6.1680000000000001</v>
       </c>
       <c r="C49">
-        <f>C48+C48*growth_rate*(1-C48/K)-B48</f>
-        <v>126.97122793230342</v>
+        <f t="shared" si="1"/>
+        <v>128.55116641339768</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -2577,8 +2636,8 @@
         <v>9.3789999999999996</v>
       </c>
       <c r="C50">
-        <f>C49+C49*growth_rate*(1-C49/K)-B49</f>
-        <v>130.1470325611167</v>
+        <f t="shared" si="1"/>
+        <v>131.86113072595774</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -2589,8 +2648,8 @@
         <v>5.23</v>
       </c>
       <c r="C51">
-        <f>C50+C50*growth_rate*(1-C50/K)-B50</f>
-        <v>128.90894135786419</v>
+        <f t="shared" si="1"/>
+        <v>130.76165581889506</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -2601,8 +2660,8 @@
         <v>3.133</v>
       </c>
       <c r="C52">
-        <f>C51+C51*growth_rate*(1-C51/K)-B51</f>
-        <v>132.29713907986564</v>
+        <f t="shared" si="1"/>
+        <v>134.21730030310363</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -2613,8 +2672,8 @@
         <v>17</v>
       </c>
       <c r="C53">
-        <f>C52+C52*growth_rate*(1-C52/K)-B52</f>
-        <v>136.45085273331935</v>
+        <f t="shared" si="1"/>
+        <v>138.46660396357177</v>
       </c>
     </row>
     <row r="54" spans="1:3">
@@ -2622,8 +2681,8 @@
         <v>2014</v>
       </c>
       <c r="C54">
-        <f>C53+C53*growth_rate*(1-C53/K)-B53</f>
-        <v>124.99636743068837</v>
+        <f t="shared" si="1"/>
+        <v>127.13802056748773</v>
       </c>
     </row>
   </sheetData>
@@ -2642,7 +2701,7 @@
   <dimension ref="A1:K59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2653,10 +2712,10 @@
       </c>
       <c r="B1">
         <f>EXP(C1)</f>
-        <v>0.51491040393046406</v>
+        <v>0.4985889849969628</v>
       </c>
       <c r="C1">
-        <v>-0.66376236640400532</v>
+        <v>-0.69597319999999996</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -2665,10 +2724,10 @@
       </c>
       <c r="B2">
         <f>EXP(C2)</f>
-        <v>148.14360792155884</v>
+        <v>150.85961463986357</v>
       </c>
       <c r="C2">
-        <v>4.9981821270986062</v>
+        <v>5.0163497000000001</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -2677,10 +2736,10 @@
       </c>
       <c r="B3">
         <f>K*EXP(C3)</f>
-        <v>151.08377126528265</v>
+        <v>179.85300889019641</v>
       </c>
       <c r="C3">
-        <v>1.9652332475952859E-2</v>
+        <v>0.17579020000000001</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -2689,7 +2748,7 @@
       </c>
       <c r="B4">
         <f>InitBio/K</f>
-        <v>1.0198467108029434</v>
+        <v>1.1921879113873299</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -2698,7 +2757,7 @@
       </c>
       <c r="B5">
         <f>EXP((1/B7)*SUM(I10:I59))</f>
-        <v>1.0097815658209293</v>
+        <v>0.98340741753763516</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -2707,7 +2766,7 @@
       </c>
       <c r="B6">
         <f>SQRT(SUMPRODUCT(K10:K59,K10:K59)/B7)</f>
-        <v>0.18478432988960355</v>
+        <v>0.18413586983409375</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -2725,7 +2784,7 @@
       </c>
       <c r="B8">
         <f>B7*LN(sigma)+B7/2</f>
-        <v>-49.91976857026016</v>
+        <v>-50.067417576200029</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2762,11 +2821,11 @@
         <v/>
       </c>
       <c r="J10" t="str">
-        <f>IF(G10="","",H10*q)</f>
+        <f t="shared" ref="J10:J41" si="0">IF(G10="","",H10*q)</f>
         <v/>
       </c>
       <c r="K10" t="str">
-        <f>IF(G10="","",LN(G10/J10))</f>
+        <f t="shared" ref="K10:K41" si="1">IF(G10="","",LN(G10/J10))</f>
         <v/>
       </c>
     </row>
@@ -2780,15 +2839,15 @@
         <v/>
       </c>
       <c r="I11" t="str">
-        <f t="shared" ref="I11:I59" si="0">IF(G11="","",LN(G11/H11))</f>
+        <f t="shared" ref="I11:I59" si="2">IF(G11="","",LN(G11/H11))</f>
         <v/>
       </c>
       <c r="J11" t="str">
-        <f>IF(G11="","",H11*q)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K11" t="str">
-        <f>IF(G11="","",LN(G11/J11))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2802,15 +2861,15 @@
         <v/>
       </c>
       <c r="I12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J12" t="str">
-        <f>IF(G12="","",H12*q)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K12" t="str">
-        <f>IF(G12="","",LN(G12/J12))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2824,15 +2883,15 @@
         <v/>
       </c>
       <c r="I13" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J13" t="str">
-        <f>IF(G13="","",H13*q)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K13" t="str">
-        <f>IF(G13="","",LN(G13/J13))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2846,15 +2905,15 @@
         <v/>
       </c>
       <c r="I14" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J14" t="str">
-        <f>IF(G14="","",H14*q)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K14" t="str">
-        <f>IF(G14="","",LN(G14/J14))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2868,15 +2927,15 @@
         <v/>
       </c>
       <c r="I15" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J15" t="str">
-        <f>IF(G15="","",H15*q)</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="K15" t="str">
-        <f>IF(G15="","",LN(G15/J15))</f>
+        <f t="shared" si="1"/>
         <v/>
       </c>
     </row>
@@ -2889,19 +2948,19 @@
       </c>
       <c r="H16">
         <f>IF(G16="","",AVERAGE(Model!C11:C12))</f>
-        <v>95.219763642387704</v>
+        <v>97.793481896723222</v>
       </c>
       <c r="I16">
-        <f t="shared" si="0"/>
-        <v>2.0496506380279465E-2</v>
+        <f t="shared" si="2"/>
+        <v>-6.1738996299554507E-3</v>
       </c>
       <c r="J16">
-        <f>IF(G16="","",H16*q)</f>
-        <v>96.151162027909052</v>
+        <f t="shared" si="0"/>
+        <v>96.170835484070054</v>
       </c>
       <c r="K16">
-        <f>IF(G16="","",LN(G16/J16))</f>
-        <v>1.0762470381583573E-2</v>
+        <f t="shared" si="1"/>
+        <v>1.0557881655549804E-2</v>
       </c>
     </row>
     <row r="17" spans="6:11">
@@ -2913,19 +2972,19 @@
       </c>
       <c r="H17">
         <f>IF(G17="","",AVERAGE(Model!C12:C13))</f>
-        <v>74.020220025280821</v>
+        <v>76.23547433930483</v>
       </c>
       <c r="I17">
-        <f t="shared" si="0"/>
-        <v>7.0642508375862639E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.1153910968810117E-2</v>
       </c>
       <c r="J17">
-        <f>IF(G17="","",H17*q)</f>
-        <v>74.744253679537778</v>
+        <f t="shared" si="0"/>
+        <v>74.97053094477242</v>
       </c>
       <c r="K17">
-        <f>IF(G17="","",LN(G17/J17))</f>
-        <v>6.0908472377166567E-2</v>
+        <f t="shared" si="1"/>
+        <v>5.7885692254315266E-2</v>
       </c>
     </row>
     <row r="18" spans="6:11">
@@ -2937,19 +2996,19 @@
       </c>
       <c r="H18">
         <f>IF(G18="","",AVERAGE(Model!C13:C14))</f>
-        <v>56.68634929346009</v>
+        <v>58.640602727311425</v>
       </c>
       <c r="I18">
-        <f t="shared" si="0"/>
-        <v>-8.9071138011557624E-2</v>
+        <f t="shared" si="2"/>
+        <v>-0.12296504542389625</v>
       </c>
       <c r="J18">
-        <f>IF(G18="","",H18*q)</f>
-        <v>57.240830550222256</v>
+        <f t="shared" si="0"/>
+        <v>57.667603690915733</v>
       </c>
       <c r="K18">
-        <f>IF(G18="","",LN(G18/J18))</f>
-        <v>-9.8805174010253641E-2</v>
+        <f t="shared" si="1"/>
+        <v>-0.10623326413839121</v>
       </c>
     </row>
     <row r="19" spans="6:11">
@@ -2961,19 +3020,19 @@
       </c>
       <c r="H19">
         <f>IF(G19="","",AVERAGE(Model!C14:C15))</f>
-        <v>45.968825619179491</v>
+        <v>47.779869209910288</v>
       </c>
       <c r="I19">
-        <f t="shared" si="0"/>
-        <v>-0.12860748484016418</v>
+        <f t="shared" si="2"/>
+        <v>-0.16724842658130529</v>
       </c>
       <c r="J19">
-        <f>IF(G19="","",H19*q)</f>
-        <v>46.418472712684313</v>
+        <f t="shared" si="0"/>
+        <v>46.987077790003845</v>
       </c>
       <c r="K19">
-        <f>IF(G19="","",LN(G19/J19))</f>
-        <v>-0.13834152083886014</v>
+        <f t="shared" si="1"/>
+        <v>-0.15051664529580019</v>
       </c>
     </row>
     <row r="20" spans="6:11">
@@ -2985,19 +3044,19 @@
       </c>
       <c r="H20">
         <f>IF(G20="","",AVERAGE(Model!C15:C16))</f>
-        <v>38.643873404784117</v>
+        <v>40.408583232133452</v>
       </c>
       <c r="I20">
-        <f t="shared" si="0"/>
-        <v>-2.9713034274532972E-2</v>
+        <f t="shared" si="2"/>
+        <v>-7.4367005201615363E-2</v>
       </c>
       <c r="J20">
-        <f>IF(G20="","",H20*q)</f>
-        <v>39.021870996068671</v>
+        <f t="shared" si="0"/>
+        <v>39.738100482666944</v>
       </c>
       <c r="K20">
-        <f>IF(G20="","",LN(G20/J20))</f>
-        <v>-3.9447070273228975E-2</v>
+        <f t="shared" si="1"/>
+        <v>-5.7635223916110249E-2</v>
       </c>
     </row>
     <row r="21" spans="6:11">
@@ -3009,19 +3068,19 @@
       </c>
       <c r="H21">
         <f>IF(G21="","",AVERAGE(Model!C16:C17))</f>
-        <v>37.829303305795676</v>
+        <v>39.639303565920287</v>
       </c>
       <c r="I21">
-        <f t="shared" si="0"/>
-        <v>0.10042161579707987</v>
+        <f t="shared" si="2"/>
+        <v>5.3684497490351091E-2</v>
       </c>
       <c r="J21">
-        <f>IF(G21="","",H21*q)</f>
-        <v>38.199333126041211</v>
+        <f t="shared" si="0"/>
+        <v>38.981585152752039</v>
       </c>
       <c r="K21">
-        <f>IF(G21="","",LN(G21/J21))</f>
-        <v>9.0687579798383933E-2</v>
+        <f t="shared" si="1"/>
+        <v>7.0416278775856198E-2</v>
       </c>
     </row>
     <row r="22" spans="6:11">
@@ -3033,19 +3092,19 @@
       </c>
       <c r="H22">
         <f>IF(G22="","",AVERAGE(Model!C17:C18))</f>
-        <v>42.458264704884996</v>
+        <v>44.334689708960227</v>
       </c>
       <c r="I22">
-        <f t="shared" si="0"/>
-        <v>0.42887019241416086</v>
+        <f t="shared" si="2"/>
+        <v>0.385624344891355</v>
       </c>
       <c r="J22">
-        <f>IF(G22="","",H22*q)</f>
-        <v>42.873573015738266</v>
+        <f t="shared" si="0"/>
+        <v>43.599062714020945</v>
       </c>
       <c r="K22">
-        <f>IF(G22="","",LN(G22/J22))</f>
-        <v>0.41913615641546487</v>
+        <f t="shared" si="1"/>
+        <v>0.40235612617686006</v>
       </c>
     </row>
     <row r="23" spans="6:11">
@@ -3057,19 +3116,19 @@
       </c>
       <c r="H23">
         <f>IF(G23="","",AVERAGE(Model!C18:C19))</f>
-        <v>44.491722660345495</v>
+        <v>46.380658594727649</v>
       </c>
       <c r="I23">
-        <f t="shared" si="0"/>
-        <v>-1.3139781665551852E-3</v>
+        <f t="shared" si="2"/>
+        <v>-4.2893345627745147E-2</v>
       </c>
       <c r="J23">
-        <f>IF(G23="","",H23*q)</f>
-        <v>44.926921374034194</v>
+        <f t="shared" si="0"/>
+        <v>45.611083692335839</v>
       </c>
       <c r="K23">
-        <f>IF(G23="","",LN(G23/J23))</f>
-        <v>-1.1048014165251177E-2</v>
+        <f t="shared" si="1"/>
+        <v>-2.6161564342240009E-2</v>
       </c>
     </row>
     <row r="24" spans="6:11">
@@ -3081,19 +3140,19 @@
       </c>
       <c r="H24">
         <f>IF(G24="","",AVERAGE(Model!C19:C20))</f>
-        <v>43.611950195083963</v>
+        <v>45.487263852840556</v>
       </c>
       <c r="I24">
-        <f t="shared" si="0"/>
-        <v>-0.12166844952916998</v>
+        <f t="shared" si="2"/>
+        <v>-0.16376962113707594</v>
       </c>
       <c r="J24">
-        <f>IF(G24="","",H24*q)</f>
-        <v>44.038543356496263</v>
+        <f t="shared" si="0"/>
+        <v>44.732512676374952</v>
       </c>
       <c r="K24">
-        <f>IF(G24="","",LN(G24/J24))</f>
-        <v>-0.13140248552786588</v>
+        <f t="shared" si="1"/>
+        <v>-0.14703783985157076</v>
       </c>
     </row>
     <row r="25" spans="6:11">
@@ -3105,19 +3164,19 @@
       </c>
       <c r="H25">
         <f>IF(G25="","",AVERAGE(Model!C20:C21))</f>
-        <v>44.088832815994515</v>
+        <v>45.960069661057034</v>
       </c>
       <c r="I25">
-        <f t="shared" si="0"/>
-        <v>0.15643615522236909</v>
+        <f t="shared" si="2"/>
+        <v>0.11486971281321653</v>
       </c>
       <c r="J25">
-        <f>IF(G25="","",H25*q)</f>
-        <v>44.520090636152112</v>
+        <f t="shared" si="0"/>
+        <v>45.197473415229915</v>
       </c>
       <c r="K25">
-        <f>IF(G25="","",LN(G25/J25))</f>
-        <v>0.14670211922367307</v>
+        <f t="shared" si="1"/>
+        <v>0.13160149409872166</v>
       </c>
     </row>
     <row r="26" spans="6:11">
@@ -3129,19 +3188,19 @@
       </c>
       <c r="H26">
         <f>IF(G26="","",AVERAGE(Model!C21:C22))</f>
-        <v>46.49684825247293</v>
+        <v>48.356900337040422</v>
       </c>
       <c r="I26">
-        <f t="shared" si="0"/>
-        <v>-2.971753198884574E-2</v>
+        <f t="shared" si="2"/>
+        <v>-6.8941929307065428E-2</v>
       </c>
       <c r="J26">
-        <f>IF(G26="","",H26*q)</f>
-        <v>46.951660234120254</v>
+        <f t="shared" si="0"/>
+        <v>47.554534480573722</v>
       </c>
       <c r="K26">
-        <f>IF(G26="","",LN(G26/J26))</f>
-        <v>-3.9451567987541798E-2</v>
+        <f t="shared" si="1"/>
+        <v>-5.2210148021560369E-2</v>
       </c>
     </row>
     <row r="27" spans="6:11">
@@ -3153,19 +3212,19 @@
       </c>
       <c r="H27">
         <f>IF(G27="","",AVERAGE(Model!C22:C23))</f>
-        <v>48.922430154870447</v>
+        <v>50.737260102107712</v>
       </c>
       <c r="I27">
-        <f t="shared" si="0"/>
-        <v>-0.12370847955634885</v>
+        <f t="shared" si="2"/>
+        <v>-0.16013304780718704</v>
       </c>
       <c r="J27">
-        <f>IF(G27="","",H27*q)</f>
-        <v>49.400968125550129</v>
+        <f t="shared" si="0"/>
+        <v>49.895397929949034</v>
       </c>
       <c r="K27">
-        <f>IF(G27="","",LN(G27/J27))</f>
-        <v>-0.13344251555504488</v>
+        <f t="shared" si="1"/>
+        <v>-0.143401266521682</v>
       </c>
     </row>
     <row r="28" spans="6:11">
@@ -3177,19 +3236,19 @@
       </c>
       <c r="H28">
         <f>IF(G28="","",AVERAGE(Model!C23:C24))</f>
-        <v>53.888992285548582</v>
+        <v>55.621909825745767</v>
       </c>
       <c r="I28">
-        <f t="shared" si="0"/>
-        <v>0.10741832992177598</v>
+        <f t="shared" si="2"/>
+        <v>7.5767376973318243E-2</v>
       </c>
       <c r="J28">
-        <f>IF(G28="","",H28*q)</f>
-        <v>54.416111010613221</v>
+        <f t="shared" si="0"/>
+        <v>54.698998700247863</v>
       </c>
       <c r="K28">
-        <f>IF(G28="","",LN(G28/J28))</f>
-        <v>9.7684293923080215E-2</v>
+        <f t="shared" si="1"/>
+        <v>9.2499158258823155E-2</v>
       </c>
     </row>
     <row r="29" spans="6:11">
@@ -3201,19 +3260,19 @@
       </c>
       <c r="H29">
         <f>IF(G29="","",AVERAGE(Model!C24:C25))</f>
-        <v>57.900621062168476</v>
+        <v>59.489772450829314</v>
       </c>
       <c r="I29">
-        <f t="shared" si="0"/>
-        <v>0.44756777793283881</v>
+        <f t="shared" si="2"/>
+        <v>0.42049148272275066</v>
       </c>
       <c r="J29">
-        <f>IF(G29="","",H29*q)</f>
-        <v>58.466979798160757</v>
+        <f t="shared" si="0"/>
+        <v>58.502683495771606</v>
       </c>
       <c r="K29">
-        <f>IF(G29="","",LN(G29/J29))</f>
-        <v>0.43783374193414287</v>
+        <f t="shared" si="1"/>
+        <v>0.43722326400825579</v>
       </c>
     </row>
     <row r="30" spans="6:11">
@@ -3225,19 +3284,19 @@
       </c>
       <c r="H30">
         <f>IF(G30="","",AVERAGE(Model!C25:C26))</f>
-        <v>53.211277431812832</v>
+        <v>54.604136407524223</v>
       </c>
       <c r="I30">
-        <f t="shared" si="0"/>
-        <v>0.10934536869467142</v>
+        <f t="shared" si="2"/>
+        <v>8.3506086117393269E-2</v>
       </c>
       <c r="J30">
-        <f>IF(G30="","",H30*q)</f>
-        <v>53.731767044427833</v>
+        <f t="shared" si="0"/>
+        <v>53.698112771396161</v>
       </c>
       <c r="K30">
-        <f>IF(G30="","",LN(G30/J30))</f>
-        <v>9.9611332695975524E-2</v>
+        <f t="shared" si="1"/>
+        <v>0.10023786740289836</v>
       </c>
     </row>
     <row r="31" spans="6:11">
@@ -3249,19 +3308,19 @@
       </c>
       <c r="H31">
         <f>IF(G31="","",AVERAGE(Model!C26:C27))</f>
-        <v>41.099437827133315</v>
+        <v>42.306616039350004</v>
       </c>
       <c r="I31">
-        <f t="shared" si="0"/>
-        <v>-3.8772949829997086E-2</v>
+        <f t="shared" si="2"/>
+        <v>-6.7721987964786262E-2</v>
       </c>
       <c r="J31">
-        <f>IF(G31="","",H31*q)</f>
-        <v>41.50145468344261</v>
+        <f t="shared" si="0"/>
+        <v>41.604640024013484</v>
       </c>
       <c r="K31">
-        <f>IF(G31="","",LN(G31/J31))</f>
-        <v>-4.8506985828693082E-2</v>
+        <f t="shared" si="1"/>
+        <v>-5.0990206679281232E-2</v>
       </c>
     </row>
     <row r="32" spans="6:11">
@@ -3273,19 +3332,19 @@
       </c>
       <c r="H32">
         <f>IF(G32="","",AVERAGE(Model!C27:C28))</f>
-        <v>32.98757834336034</v>
+        <v>34.085696023743608</v>
       </c>
       <c r="I32">
-        <f t="shared" si="0"/>
-        <v>-2.2193052279946335E-2</v>
+        <f t="shared" si="2"/>
+        <v>-5.4939800354747999E-2</v>
       </c>
       <c r="J32">
-        <f>IF(G32="","",H32*q)</f>
-        <v>33.310248512198982</v>
+        <f t="shared" si="0"/>
+        <v>33.520126301682538</v>
       </c>
       <c r="K32">
-        <f>IF(G32="","",LN(G32/J32))</f>
-        <v>-3.1927088278642442E-2</v>
+        <f t="shared" si="1"/>
+        <v>-3.8208019069242836E-2</v>
       </c>
     </row>
     <row r="33" spans="6:11">
@@ -3297,19 +3356,19 @@
       </c>
       <c r="H33">
         <f>IF(G33="","",AVERAGE(Model!C28:C29))</f>
-        <v>29.948516389043824</v>
+        <v>30.998192354718054</v>
       </c>
       <c r="I33">
-        <f t="shared" si="0"/>
-        <v>-0.28696101434555815</v>
+        <f t="shared" si="2"/>
+        <v>-0.32141011891688992</v>
       </c>
       <c r="J33">
-        <f>IF(G33="","",H33*q)</f>
-        <v>30.241459773342434</v>
+        <f t="shared" si="0"/>
+        <v>30.483852291888148</v>
       </c>
       <c r="K33">
-        <f>IF(G33="","",LN(G33/J33))</f>
-        <v>-0.29669505034425403</v>
+        <f t="shared" si="1"/>
+        <v>-0.30467833763138491</v>
       </c>
     </row>
     <row r="34" spans="6:11">
@@ -3321,19 +3380,19 @@
       </c>
       <c r="H34">
         <f>IF(G34="","",AVERAGE(Model!C29:C30))</f>
-        <v>29.059615043904532</v>
+        <v>30.085832449377989</v>
       </c>
       <c r="I34">
-        <f t="shared" si="0"/>
-        <v>0.18741588051203192</v>
+        <f t="shared" si="2"/>
+        <v>0.15271091342175261</v>
       </c>
       <c r="J34">
-        <f>IF(G34="","",H34*q)</f>
-        <v>29.34386358118735</v>
+        <f t="shared" si="0"/>
+        <v>29.586630793512793</v>
       </c>
       <c r="K34">
-        <f>IF(G34="","",LN(G34/J34))</f>
-        <v>0.17768184451333596</v>
+        <f t="shared" si="1"/>
+        <v>0.1694426947072577</v>
       </c>
     </row>
     <row r="35" spans="6:11">
@@ -3345,19 +3404,19 @@
       </c>
       <c r="H35">
         <f>IF(G35="","",AVERAGE(Model!C30:C31))</f>
-        <v>28.988926220547164</v>
+        <v>29.996239931462277</v>
       </c>
       <c r="I35">
-        <f t="shared" si="0"/>
-        <v>-0.13622449655752913</v>
+        <f t="shared" si="2"/>
+        <v>-0.17038263214899324</v>
       </c>
       <c r="J35">
-        <f>IF(G35="","",H35*q)</f>
-        <v>29.272483310451509</v>
+        <f t="shared" si="0"/>
+        <v>29.49852484683861</v>
       </c>
       <c r="K35">
-        <f>IF(G35="","",LN(G35/J35))</f>
-        <v>-0.14595853255622518</v>
+        <f t="shared" si="1"/>
+        <v>-0.15365085086348818</v>
       </c>
     </row>
     <row r="36" spans="6:11">
@@ -3369,19 +3428,19 @@
       </c>
       <c r="H36">
         <f>IF(G36="","",AVERAGE(Model!C31:C32))</f>
-        <v>25.897697539299966</v>
+        <v>26.881277971605915</v>
       </c>
       <c r="I36">
-        <f t="shared" si="0"/>
-        <v>1.0456154416241278E-2</v>
+        <f t="shared" si="2"/>
+        <v>-2.6819837037780889E-2</v>
       </c>
       <c r="J36">
-        <f>IF(G36="","",H36*q)</f>
-        <v>26.151017572391147</v>
+        <f t="shared" si="0"/>
+        <v>26.435248150168292</v>
       </c>
       <c r="K36">
-        <f>IF(G36="","",LN(G36/J36))</f>
-        <v>7.2211841754540157E-4</v>
+        <f t="shared" si="1"/>
+        <v>-1.0088055752275739E-2</v>
       </c>
     </row>
     <row r="37" spans="6:11">
@@ -3393,19 +3452,19 @@
       </c>
       <c r="H37">
         <f>IF(G37="","",AVERAGE(Model!C32:C33))</f>
-        <v>23.401687764925775</v>
+        <v>24.396670387622272</v>
       </c>
       <c r="I37">
-        <f t="shared" si="0"/>
-        <v>-0.17458983072473835</v>
+        <f t="shared" si="2"/>
+        <v>-0.21622834771988955</v>
       </c>
       <c r="J37">
-        <f>IF(G37="","",H37*q)</f>
-        <v>23.63059291411923</v>
+        <f t="shared" si="0"/>
+        <v>23.991866622408516</v>
       </c>
       <c r="K37">
-        <f>IF(G37="","",LN(G37/J37))</f>
-        <v>-0.18432386672343429</v>
+        <f t="shared" si="1"/>
+        <v>-0.19949656643438449</v>
       </c>
     </row>
     <row r="38" spans="6:11">
@@ -3417,19 +3476,19 @@
       </c>
       <c r="H38">
         <f>IF(G38="","",AVERAGE(Model!C33:C34))</f>
-        <v>21.35926477879832</v>
+        <v>22.404768349096919</v>
       </c>
       <c r="I38">
-        <f t="shared" si="0"/>
-        <v>0.40990114971408115</v>
+        <f t="shared" si="2"/>
+        <v>0.36211293381108284</v>
       </c>
       <c r="J38">
-        <f>IF(G38="","",H38*q)</f>
-        <v>21.568191833118792</v>
+        <f t="shared" si="0"/>
+        <v>22.033015382714346</v>
       </c>
       <c r="K38">
-        <f>IF(G38="","",LN(G38/J38))</f>
-        <v>0.4001671137153851</v>
+        <f t="shared" si="1"/>
+        <v>0.3788447150965879</v>
       </c>
     </row>
     <row r="39" spans="6:11">
@@ -3441,19 +3500,19 @@
       </c>
       <c r="H39">
         <f>IF(G39="","",AVERAGE(Model!C34:C35))</f>
-        <v>22.918651544431526</v>
+        <v>24.064401423566487</v>
       </c>
       <c r="I39">
-        <f t="shared" si="0"/>
-        <v>9.9592493672596316E-2</v>
+        <f t="shared" si="2"/>
+        <v>5.0809921522175151E-2</v>
       </c>
       <c r="J39">
-        <f>IF(G39="","",H39*q)</f>
-        <v>23.142831843040327</v>
+        <f t="shared" si="0"/>
+        <v>23.665110858538512</v>
       </c>
       <c r="K39">
-        <f>IF(G39="","",LN(G39/J39))</f>
-        <v>8.9858457673900369E-2</v>
+        <f t="shared" si="1"/>
+        <v>6.7541702807680168E-2</v>
       </c>
     </row>
     <row r="40" spans="6:11">
@@ -3465,19 +3524,19 @@
       </c>
       <c r="H40">
         <f>IF(G40="","",AVERAGE(Model!C35:C36))</f>
-        <v>31.787241103567354</v>
+        <v>33.042321925452654</v>
       </c>
       <c r="I40">
-        <f t="shared" si="0"/>
-        <v>-0.3119578714098713</v>
+        <f t="shared" si="2"/>
+        <v>-0.35068210767115587</v>
       </c>
       <c r="J40">
-        <f>IF(G40="","",H40*q)</f>
-        <v>32.098170094687646</v>
+        <f t="shared" si="0"/>
+        <v>32.494064474156573</v>
       </c>
       <c r="K40">
-        <f>IF(G40="","",LN(G40/J40))</f>
-        <v>-0.32169190740856735</v>
+        <f t="shared" si="1"/>
+        <v>-0.33395032638565064</v>
       </c>
     </row>
     <row r="41" spans="6:11">
@@ -3489,19 +3548,19 @@
       </c>
       <c r="H41">
         <f>IF(G41="","",AVERAGE(Model!C36:C37))</f>
-        <v>44.387084154460133</v>
+        <v>45.656518053065703</v>
       </c>
       <c r="I41">
-        <f t="shared" si="0"/>
-        <v>-2.3487554804555964E-2</v>
+        <f t="shared" si="2"/>
+        <v>-5.1685405155421624E-2</v>
       </c>
       <c r="J41">
-        <f>IF(G41="","",H41*q)</f>
-        <v>44.821259339716114</v>
+        <f t="shared" si="0"/>
+        <v>44.898958512325763</v>
       </c>
       <c r="K41">
-        <f>IF(G41="","",LN(G41/J41))</f>
-        <v>-3.3221590803252016E-2</v>
+        <f t="shared" si="1"/>
+        <v>-3.49536238699166E-2</v>
       </c>
     </row>
     <row r="42" spans="6:11">
@@ -3513,19 +3572,19 @@
       </c>
       <c r="H42">
         <f>IF(G42="","",AVERAGE(Model!C37:C38))</f>
-        <v>59.775688545745922</v>
+        <v>60.921976917134515</v>
       </c>
       <c r="I42">
-        <f t="shared" si="0"/>
-        <v>-0.15173859981142024</v>
+        <f t="shared" si="2"/>
+        <v>-0.17073354611163677</v>
       </c>
       <c r="J42">
-        <f>IF(G42="","",H42*q)</f>
-        <v>60.360388377747505</v>
+        <f t="shared" ref="J42:J59" si="3">IF(G42="","",H42*q)</f>
+        <v>59.911123991366672</v>
       </c>
       <c r="K42">
-        <f>IF(G42="","",LN(G42/J42))</f>
-        <v>-0.16147263581011628</v>
+        <f t="shared" ref="K42:K73" si="4">IF(G42="","",LN(G42/J42))</f>
+        <v>-0.15400176482613176</v>
       </c>
     </row>
     <row r="43" spans="6:11">
@@ -3537,19 +3596,19 @@
       </c>
       <c r="H43">
         <f>IF(G43="","",AVERAGE(Model!C38:C39))</f>
-        <v>75.373040635822548</v>
+        <v>76.28530018889019</v>
       </c>
       <c r="I43">
-        <f t="shared" si="0"/>
-        <v>1.6936052839099023E-2</v>
+        <f t="shared" si="2"/>
+        <v>4.9054510126560922E-3</v>
       </c>
       <c r="J43">
-        <f>IF(G43="","",H43*q)</f>
-        <v>76.11030699392542</v>
+        <f t="shared" si="3"/>
+        <v>75.019530054839777</v>
       </c>
       <c r="K43">
-        <f>IF(G43="","",LN(G43/J43))</f>
-        <v>7.2020168404029281E-3</v>
+        <f t="shared" si="4"/>
+        <v>2.1637232298161172E-2</v>
       </c>
     </row>
     <row r="44" spans="6:11">
@@ -3561,19 +3620,19 @@
       </c>
       <c r="H44">
         <f>IF(G44="","",AVERAGE(Model!C39:C40))</f>
-        <v>88.613119176940685</v>
+        <v>89.278451855979426</v>
       </c>
       <c r="I44">
-        <f t="shared" si="0"/>
-        <v>0.25747287604244012</v>
+        <f t="shared" si="2"/>
+        <v>0.24999263650655779</v>
       </c>
       <c r="J44">
-        <f>IF(G44="","",H44*q)</f>
-        <v>89.479894234767784</v>
+        <f t="shared" si="3"/>
+        <v>87.797091781446824</v>
       </c>
       <c r="K44">
-        <f>IF(G44="","",LN(G44/J44))</f>
-        <v>0.24773884004374402</v>
+        <f t="shared" si="4"/>
+        <v>0.2667244177920628</v>
       </c>
     </row>
     <row r="45" spans="6:11">
@@ -3585,19 +3644,19 @@
       </c>
       <c r="H45">
         <f>IF(G45="","",AVERAGE(Model!C40:C41))</f>
-        <v>97.797374275644927</v>
+        <v>98.308259875564104</v>
       </c>
       <c r="I45">
-        <f t="shared" si="0"/>
-        <v>4.191102410349716E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.6700702045181346E-2</v>
       </c>
       <c r="J45">
-        <f>IF(G45="","",H45*q)</f>
-        <v>98.753985729236206</v>
+        <f t="shared" si="3"/>
+        <v>96.677071966847208</v>
       </c>
       <c r="K45">
-        <f>IF(G45="","",LN(G45/J45))</f>
-        <v>3.2176988104800998E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.3432483330686592E-2</v>
       </c>
     </row>
     <row r="46" spans="6:11">
@@ -3609,19 +3668,19 @@
       </c>
       <c r="H46">
         <f>IF(G46="","",AVERAGE(Model!C41:C42))</f>
-        <v>102.22190478163024</v>
+        <v>102.69615713061469</v>
       </c>
       <c r="I46">
-        <f t="shared" si="0"/>
-        <v>0.27513104302111357</v>
+        <f t="shared" si="2"/>
+        <v>0.27050233248876659</v>
       </c>
       <c r="J46">
-        <f>IF(G46="","",H46*q)</f>
-        <v>103.22179507159252</v>
+        <f t="shared" si="3"/>
+        <v>100.992162674857</v>
       </c>
       <c r="K46">
-        <f>IF(G46="","",LN(G46/J46))</f>
-        <v>0.26539700702241747</v>
+        <f t="shared" si="4"/>
+        <v>0.28723411377427166</v>
       </c>
     </row>
     <row r="47" spans="6:11">
@@ -3633,19 +3692,19 @@
       </c>
       <c r="H47">
         <f>IF(G47="","",AVERAGE(Model!C42:C43))</f>
-        <v>106.11128408473505</v>
+        <v>106.61696921981151</v>
       </c>
       <c r="I47">
-        <f t="shared" si="0"/>
-        <v>-0.11765973594896964</v>
+        <f t="shared" si="2"/>
+        <v>-0.1224140276778117</v>
       </c>
       <c r="J47">
-        <f>IF(G47="","",H47*q)</f>
-        <v>107.1492185943532</v>
+        <f t="shared" si="3"/>
+        <v>104.84791836614437</v>
       </c>
       <c r="K47">
-        <f>IF(G47="","",LN(G47/J47))</f>
-        <v>-0.12739377194766566</v>
+        <f t="shared" si="4"/>
+        <v>-0.10568224639230657</v>
       </c>
     </row>
     <row r="48" spans="6:11">
@@ -3657,19 +3716,19 @@
       </c>
       <c r="H48">
         <f>IF(G48="","",AVERAGE(Model!C43:C44))</f>
-        <v>109.33636583928049</v>
+        <v>109.93031368663983</v>
       </c>
       <c r="I48">
-        <f t="shared" si="0"/>
-        <v>3.9051395248520054E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.3633797815493097E-2</v>
       </c>
       <c r="J48">
-        <f>IF(G48="","",H48*q)</f>
-        <v>110.40584669835862</v>
+        <f t="shared" si="3"/>
+        <v>108.10628589168063</v>
       </c>
       <c r="K48">
-        <f>IF(G48="","",LN(G48/J48))</f>
-        <v>2.9317359249824159E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.0365579100998169E-2</v>
       </c>
     </row>
     <row r="49" spans="6:11">
@@ -3681,19 +3740,19 @@
       </c>
       <c r="H49">
         <f>IF(G49="","",AVERAGE(Model!C44:C45))</f>
-        <v>110.50313041127005</v>
+        <v>111.21948381112806</v>
       </c>
       <c r="I49">
-        <f t="shared" si="0"/>
-        <v>3.7691107057031083E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.1229376530192816E-2</v>
       </c>
       <c r="J49">
-        <f>IF(G49="","",H49*q)</f>
-        <v>111.58402405480662</v>
+        <f t="shared" si="3"/>
+        <v>109.37406535457026</v>
       </c>
       <c r="K49">
-        <f>IF(G49="","",LN(G49/J49))</f>
-        <v>2.7957071058335083E-2</v>
+        <f t="shared" si="4"/>
+        <v>4.7961157815697833E-2</v>
       </c>
     </row>
     <row r="50" spans="6:11">
@@ -3705,19 +3764,19 @@
       </c>
       <c r="H50">
         <f>IF(G50="","",AVERAGE(Model!C45:C46))</f>
-        <v>111.31525706022154</v>
+        <v>112.14528933618894</v>
       </c>
       <c r="I50">
-        <f t="shared" si="0"/>
-        <v>4.3907205698824246E-2</v>
+        <f t="shared" si="2"/>
+        <v>3.6478278250696668E-2</v>
       </c>
       <c r="J50">
-        <f>IF(G50="","",H50*q)</f>
-        <v>112.40409457402976</v>
+        <f t="shared" si="3"/>
+        <v>110.28450937511246</v>
       </c>
       <c r="K50">
-        <f>IF(G50="","",LN(G50/J50))</f>
-        <v>3.4173169700128382E-2</v>
+        <f t="shared" si="4"/>
+        <v>5.3210059536201844E-2</v>
       </c>
     </row>
     <row r="51" spans="6:11">
@@ -3729,19 +3788,19 @@
       </c>
       <c r="H51">
         <f>IF(G51="","",AVERAGE(Model!C46:C47))</f>
-        <v>118.13268621436029</v>
+        <v>119.06263006850939</v>
       </c>
       <c r="I51">
-        <f t="shared" si="0"/>
-        <v>-0.48040548468585476</v>
+        <f t="shared" si="2"/>
+        <v>-0.48824669026680023</v>
       </c>
       <c r="J51">
-        <f>IF(G51="","",H51*q)</f>
-        <v>119.28820886016923</v>
+        <f t="shared" si="3"/>
+        <v>117.08707356091161</v>
       </c>
       <c r="K51">
-        <f>IF(G51="","",LN(G51/J51))</f>
-        <v>-0.4901395206845508</v>
+        <f t="shared" si="4"/>
+        <v>-0.47151490898129506</v>
       </c>
     </row>
     <row r="52" spans="6:11">
@@ -3753,19 +3812,19 @@
       </c>
       <c r="H52">
         <f>IF(G52="","",AVERAGE(Model!C47:C48))</f>
-        <v>127.52860857602465</v>
+        <v>128.6537480110735</v>
       </c>
       <c r="I52">
-        <f t="shared" si="0"/>
-        <v>7.6082437111108792E-2</v>
+        <f t="shared" si="2"/>
+        <v>6.7298485831487162E-2</v>
       </c>
       <c r="J52">
-        <f>IF(G52="","",H52*q)</f>
-        <v>128.77603805486257</v>
+        <f t="shared" si="3"/>
+        <v>126.51905008810746</v>
       </c>
       <c r="K52">
-        <f>IF(G52="","",LN(G52/J52))</f>
-        <v>6.6348401112412608E-2</v>
+        <f t="shared" si="4"/>
+        <v>8.4030267116992338E-2</v>
       </c>
     </row>
     <row r="53" spans="6:11">
@@ -3777,19 +3836,19 @@
       </c>
       <c r="H53">
         <f>IF(G53="","",AVERAGE(Model!C48:C49))</f>
-        <v>128.62989163703097</v>
+        <v>130.05766311484456</v>
       </c>
       <c r="I53">
-        <f t="shared" si="0"/>
-        <v>-5.1809841013228546E-2</v>
+        <f t="shared" si="2"/>
+        <v>-6.2848531895006832E-2</v>
       </c>
       <c r="J53">
-        <f>IF(G53="","",H53*q)</f>
-        <v>129.88809338861759</v>
+        <f t="shared" si="3"/>
+        <v>127.89967061474904</v>
       </c>
       <c r="K53">
-        <f>IF(G53="","",LN(G53/J53))</f>
-        <v>-6.1543877011924646E-2</v>
+        <f t="shared" si="4"/>
+        <v>-4.6116750609501739E-2</v>
       </c>
     </row>
     <row r="54" spans="6:11">
@@ -3801,19 +3860,19 @@
       </c>
       <c r="H54">
         <f>IF(G54="","",AVERAGE(Model!C49:C50))</f>
-        <v>128.55913024671005</v>
+        <v>130.20614856967771</v>
       </c>
       <c r="I54">
-        <f t="shared" si="0"/>
-        <v>-0.25038299395059704</v>
+        <f t="shared" si="2"/>
+        <v>-0.2631129905903124</v>
       </c>
       <c r="J54">
-        <f>IF(G54="","",H54*q)</f>
-        <v>129.81663984109966</v>
+        <f t="shared" si="3"/>
+        <v>128.0456923124284</v>
       </c>
       <c r="K54">
-        <f>IF(G54="","",LN(G54/J54))</f>
-        <v>-0.26011702994929298</v>
+        <f t="shared" si="4"/>
+        <v>-0.24638120930480725</v>
       </c>
     </row>
     <row r="55" spans="6:11">
@@ -3825,19 +3884,19 @@
       </c>
       <c r="H55">
         <f>IF(G55="","",AVERAGE(Model!C50:C51))</f>
-        <v>129.52798695949045</v>
+        <v>131.31139327242641</v>
       </c>
       <c r="I55">
-        <f t="shared" si="0"/>
-        <v>2.8295691318908679E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.4621114253163281E-2</v>
       </c>
       <c r="J55">
-        <f>IF(G55="","",H55*q)</f>
-        <v>130.79497348958716</v>
+        <f t="shared" si="3"/>
+        <v>129.13259815130567</v>
       </c>
       <c r="K55">
-        <f>IF(G55="","",LN(G55/J55))</f>
-        <v>1.8561655320212669E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.135289553866831E-2</v>
       </c>
     </row>
     <row r="56" spans="6:11">
@@ -3849,19 +3908,19 @@
       </c>
       <c r="H56">
         <f>IF(G56="","",AVERAGE(Model!C51:C52))</f>
-        <v>130.60304021886492</v>
+        <v>132.48947806099935</v>
       </c>
       <c r="I56">
-        <f t="shared" si="0"/>
-        <v>-1.5212587304035125E-2</v>
+        <f t="shared" si="2"/>
+        <v>-2.9553323287260638E-2</v>
       </c>
       <c r="J56">
-        <f>IF(G56="","",H56*q)</f>
-        <v>131.88054245317923</v>
+        <f t="shared" si="3"/>
+        <v>130.29113547087653</v>
       </c>
       <c r="K56">
-        <f>IF(G56="","",LN(G56/J56))</f>
-        <v>-2.4946623302731234E-2</v>
+        <f t="shared" si="4"/>
+        <v>-1.2821542001755445E-2</v>
       </c>
     </row>
     <row r="57" spans="6:11">
@@ -3873,19 +3932,19 @@
       </c>
       <c r="H57">
         <f>IF(G57="","",AVERAGE(Model!C52:C53))</f>
-        <v>134.37399590659248</v>
+        <v>136.34195213333771</v>
       </c>
       <c r="I57">
-        <f t="shared" si="0"/>
-        <v>2.8982655484171574E-2</v>
+        <f t="shared" si="2"/>
+        <v>1.4443498056727429E-2</v>
       </c>
       <c r="J57">
-        <f>IF(G57="","",H57*q)</f>
-        <v>135.6883839921741</v>
+        <f t="shared" si="3"/>
+        <v>134.0796870494855</v>
       </c>
       <c r="K57">
-        <f>IF(G57="","",LN(G57/J57))</f>
-        <v>1.9248619485475602E-2</v>
+        <f t="shared" si="4"/>
+        <v>3.1175279342232496E-2</v>
       </c>
     </row>
     <row r="58" spans="6:11">
@@ -3898,15 +3957,15 @@
         <v/>
       </c>
       <c r="I58" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J58" t="str">
-        <f>IF(G58="","",H58*q)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K58" t="str">
-        <f>IF(G58="","",LN(G58/J58))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
@@ -3915,20 +3974,21 @@
         <v>2014</v>
       </c>
       <c r="I59" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="J59" t="str">
-        <f>IF(G59="","",H59*q)</f>
+        <f t="shared" si="3"/>
         <v/>
       </c>
       <c r="K59" t="str">
-        <f>IF(G59="","",LN(G59/J59))</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">

</xml_diff>